<commit_message>
Up of latest script
A1, A2, delete and feature and the main files so far
</commit_message>
<xml_diff>
--- a/criteres.xlsx
+++ b/criteres.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\m.leclech\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BillyValuation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -616,7 +616,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -630,27 +630,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -795,6 +785,22 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -809,22 +815,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:B15" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:B15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A1:B15"/>
+  <sortState ref="A2:B15">
+    <sortCondition ref="A1:A15"/>
+  </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" name="Colonne1" dataDxfId="7"/>
-    <tableColumn id="2" name="Colonne2" dataDxfId="6"/>
+    <tableColumn id="1" name="Colonne1" dataDxfId="5"/>
+    <tableColumn id="2" name="Colonne2" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="D1:E78" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="D1:E78" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <autoFilter ref="D1:E78"/>
+  <sortState ref="D2:E78">
+    <sortCondition ref="D1:D78"/>
+  </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" name="Colonne1" dataDxfId="3"/>
-    <tableColumn id="2" name="Colonne2" dataDxfId="2"/>
+    <tableColumn id="1" name="Colonne1" dataDxfId="1"/>
+    <tableColumn id="2" name="Colonne2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1095,11 +1107,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="F78" sqref="F78"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A2:A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="2" max="2" width="26.21875" customWidth="1"/>
+    <col min="5" max="5" width="30.21875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
@@ -1115,60 +1131,60 @@
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" thickBot="1">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="21" thickBot="1">
+    <row r="2" spans="1:5" ht="21" thickBot="1">
+      <c r="A2" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="31.2" thickBot="1">
       <c r="A3" s="3" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="31.2" thickBot="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="21" thickBot="1">
       <c r="A4" s="3" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="21" thickBot="1">
       <c r="A5" s="3" t="s">
-        <v>160</v>
+        <v>175</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>161</v>
+        <v>176</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="21" thickBot="1">
@@ -1179,10 +1195,10 @@
         <v>162</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>8</v>
+        <v>128</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>9</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="31.2" thickBot="1">
@@ -1249,13 +1265,13 @@
         <v>168</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>18</v>
+        <v>130</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="21" thickBot="1">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15" thickBot="1">
       <c r="A12" s="3" t="s">
         <v>169</v>
       </c>
@@ -1263,556 +1279,556 @@
         <v>170</v>
       </c>
       <c r="D12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15" thickBot="1">
+      <c r="A13" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="21" thickBot="1">
+      <c r="A14" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="31.2" thickBot="1">
-      <c r="A13" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="D13" s="3" t="s">
+    <row r="15" spans="1:5" ht="31.2" thickBot="1">
+      <c r="A15" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E15" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="31.2" thickBot="1">
-      <c r="A14" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="D14" s="3" t="s">
+    <row r="16" spans="1:5" ht="15" thickBot="1">
+      <c r="D16" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E16" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15" thickBot="1">
-      <c r="A15" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="21" thickBot="1">
-      <c r="D16" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="4:5" ht="31.2" thickBot="1">
+    <row r="17" spans="4:5" ht="15" thickBot="1">
       <c r="D17" s="3" t="s">
-        <v>30</v>
+        <v>150</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>31</v>
+        <v>151</v>
       </c>
     </row>
     <row r="18" spans="4:5" ht="15" thickBot="1">
       <c r="D18" s="3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="4:5" ht="15" thickBot="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="4:5" ht="21" thickBot="1">
       <c r="D19" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="4:5" ht="15" thickBot="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="4:5" ht="31.2" thickBot="1">
       <c r="D20" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="4:5" ht="15" thickBot="1">
       <c r="D21" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="4:5" ht="15" thickBot="1">
+      <c r="D22" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="4:5" ht="41.4" thickBot="1">
+      <c r="D23" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="24" spans="4:5" ht="15" thickBot="1">
+      <c r="D24" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="4:5" ht="31.2" thickBot="1">
+      <c r="D25" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="26" spans="4:5" ht="15" thickBot="1">
+      <c r="D26" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E26" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="4:5" ht="41.4" thickBot="1">
-      <c r="D22" s="3" t="s">
+    <row r="27" spans="4:5" ht="15" thickBot="1">
+      <c r="D27" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="28" spans="4:5" ht="41.4" thickBot="1">
+      <c r="D28" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E28" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="4:5" ht="15" thickBot="1">
-      <c r="D23" s="3" t="s">
+    <row r="29" spans="4:5" ht="15" thickBot="1">
+      <c r="D29" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E29" s="4" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="4:5" ht="41.4" thickBot="1">
-      <c r="D24" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="4:5" ht="21" thickBot="1">
-      <c r="D25" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="26" spans="4:5" ht="21" thickBot="1">
-      <c r="D26" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="27" spans="4:5" ht="21" thickBot="1">
-      <c r="D27" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="28" spans="4:5" ht="21" thickBot="1">
-      <c r="D28" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="29" spans="4:5" ht="41.4" thickBot="1">
-      <c r="D29" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="30" spans="4:5" ht="15" thickBot="1">
       <c r="D30" s="3" t="s">
-        <v>56</v>
+        <v>138</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="31" spans="4:5" ht="21" thickBot="1">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="31" spans="4:5" ht="31.2" thickBot="1">
       <c r="D31" s="3" t="s">
-        <v>58</v>
+        <v>140</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="32" spans="4:5" ht="31.2" thickBot="1">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="32" spans="4:5" ht="41.4" thickBot="1">
       <c r="D32" s="3" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="33" spans="4:5" ht="31.2" thickBot="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="4:5" ht="21" thickBot="1">
       <c r="D33" s="3" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="4:5" ht="21" thickBot="1">
       <c r="D34" s="3" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="4:5" ht="21" thickBot="1">
       <c r="D35" s="3" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="4:5" ht="21" thickBot="1">
       <c r="D36" s="3" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="37" spans="4:5" ht="31.2" thickBot="1">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="4:5" ht="21" thickBot="1">
       <c r="D37" s="3" t="s">
-        <v>70</v>
+        <v>142</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>71</v>
+        <v>143</v>
       </c>
     </row>
     <row r="38" spans="4:5" ht="21" thickBot="1">
       <c r="D38" s="3" t="s">
-        <v>72</v>
+        <v>144</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>73</v>
+        <v>145</v>
       </c>
     </row>
     <row r="39" spans="4:5" ht="21" thickBot="1">
       <c r="D39" s="3" t="s">
-        <v>74</v>
+        <v>146</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="40" spans="4:5" ht="21" thickBot="1">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="40" spans="4:5" ht="41.4" thickBot="1">
       <c r="D40" s="3" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="41" spans="4:5" ht="21" thickBot="1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="4:5" ht="15" thickBot="1">
       <c r="D41" s="3" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="42" spans="4:5" ht="15" thickBot="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="42" spans="4:5" ht="21" thickBot="1">
       <c r="D42" s="3" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="43" spans="4:5" ht="15" thickBot="1">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="43" spans="4:5" ht="31.2" thickBot="1">
       <c r="D43" s="3" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="44" spans="4:5" ht="15" thickBot="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="44" spans="4:5" ht="31.2" thickBot="1">
       <c r="D44" s="3" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
     </row>
     <row r="45" spans="4:5" ht="21" thickBot="1">
       <c r="D45" s="3" t="s">
-        <v>86</v>
+        <v>148</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="46" spans="4:5" ht="41.4" thickBot="1">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="46" spans="4:5" ht="21" thickBot="1">
       <c r="D46" s="3" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="47" spans="4:5" ht="15" thickBot="1">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="47" spans="4:5" ht="21" thickBot="1">
       <c r="D47" s="3" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="48" spans="4:5" ht="31.2" thickBot="1">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="48" spans="4:5" ht="21" thickBot="1">
       <c r="D48" s="3" t="s">
-        <v>92</v>
+        <v>68</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="49" spans="4:5" ht="21" thickBot="1">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="49" spans="4:5" ht="31.2" thickBot="1">
       <c r="D49" s="3" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
     </row>
     <row r="50" spans="4:5" ht="21" thickBot="1">
       <c r="D50" s="3" t="s">
-        <v>96</v>
+        <v>72</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
     </row>
     <row r="51" spans="4:5" ht="21" thickBot="1">
       <c r="D51" s="3" t="s">
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="52" spans="4:5" ht="31.2" thickBot="1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="52" spans="4:5" ht="21" thickBot="1">
       <c r="D52" s="3" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="53" spans="4:5" ht="15" thickBot="1">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="53" spans="4:5" ht="21" thickBot="1">
       <c r="D53" s="3" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
     </row>
     <row r="54" spans="4:5" ht="15" thickBot="1">
       <c r="D54" s="3" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
     </row>
     <row r="55" spans="4:5" ht="15" thickBot="1">
       <c r="D55" s="3" t="s">
-        <v>106</v>
+        <v>82</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
     </row>
     <row r="56" spans="4:5" ht="15" thickBot="1">
       <c r="D56" s="3" t="s">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
     </row>
     <row r="57" spans="4:5" ht="21" thickBot="1">
       <c r="D57" s="3" t="s">
-        <v>110</v>
+        <v>86</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="58" spans="4:5" ht="15" thickBot="1">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="58" spans="4:5" ht="41.4" thickBot="1">
       <c r="D58" s="3" t="s">
-        <v>112</v>
+        <v>88</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="59" spans="4:5" ht="21" thickBot="1">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="59" spans="4:5" ht="15" thickBot="1">
       <c r="D59" s="3" t="s">
-        <v>114</v>
+        <v>90</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="60" spans="4:5" ht="15" thickBot="1">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="60" spans="4:5" ht="31.2" thickBot="1">
       <c r="D60" s="3" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="61" spans="4:5" ht="51.6" thickBot="1">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="61" spans="4:5" ht="21" thickBot="1">
       <c r="D61" s="3" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="62" spans="4:5" ht="15" thickBot="1">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="62" spans="4:5" ht="21" thickBot="1">
       <c r="D62" s="3" t="s">
-        <v>120</v>
+        <v>96</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>121</v>
+        <v>97</v>
       </c>
     </row>
     <row r="63" spans="4:5" ht="21" thickBot="1">
       <c r="D63" s="3" t="s">
-        <v>122</v>
+        <v>98</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="64" spans="4:5" ht="15" thickBot="1">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="64" spans="4:5" ht="31.2" thickBot="1">
       <c r="D64" s="3" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
     </row>
     <row r="65" spans="4:5" ht="15" thickBot="1">
       <c r="D65" s="3" t="s">
-        <v>126</v>
+        <v>102</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="66" spans="4:5" ht="21" thickBot="1">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="66" spans="4:5" ht="15" thickBot="1">
       <c r="D66" s="3" t="s">
-        <v>128</v>
+        <v>104</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="67" spans="4:5" ht="21" thickBot="1">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="67" spans="4:5" ht="15" thickBot="1">
       <c r="D67" s="3" t="s">
-        <v>130</v>
+        <v>106</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>131</v>
+        <v>107</v>
       </c>
     </row>
     <row r="68" spans="4:5" ht="15" thickBot="1">
       <c r="D68" s="3" t="s">
-        <v>132</v>
+        <v>108</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="69" spans="4:5" ht="31.2" thickBot="1">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="69" spans="4:5" ht="21" thickBot="1">
       <c r="D69" s="3" t="s">
-        <v>134</v>
+        <v>110</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>135</v>
+        <v>111</v>
       </c>
     </row>
     <row r="70" spans="4:5" ht="15" thickBot="1">
       <c r="D70" s="3" t="s">
-        <v>136</v>
+        <v>112</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>137</v>
+        <v>113</v>
       </c>
     </row>
     <row r="71" spans="4:5" ht="15" thickBot="1">
       <c r="D71" s="3" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="72" spans="4:5" ht="31.2" thickBot="1">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="72" spans="4:5" ht="15" thickBot="1">
       <c r="D72" s="3" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
     </row>
     <row r="73" spans="4:5" ht="21" thickBot="1">
       <c r="D73" s="3" t="s">
-        <v>142</v>
+        <v>114</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="74" spans="4:5" ht="21" thickBot="1">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="74" spans="4:5" ht="15" thickBot="1">
       <c r="D74" s="3" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="75" spans="4:5" ht="21" thickBot="1">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="75" spans="4:5" ht="15" thickBot="1">
       <c r="D75" s="3" t="s">
-        <v>146</v>
+        <v>0</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="76" spans="4:5" ht="21" thickBot="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="4:5" ht="51.6" thickBot="1">
       <c r="D76" s="3" t="s">
-        <v>148</v>
+        <v>118</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>149</v>
+        <v>119</v>
       </c>
     </row>
     <row r="77" spans="4:5" ht="15" thickBot="1">
       <c r="D77" s="3" t="s">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="78" spans="4:5" ht="40.799999999999997">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="78" spans="4:5" ht="20.399999999999999">
       <c r="D78" s="3" t="s">
-        <v>152</v>
+        <v>122</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>153</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>